<commit_message>
Canola - Inconsistent capitalisation between observed files
</commit_message>
<xml_diff>
--- a/Tests/Validation/Canola/Greenethorpe2013.xlsx
+++ b/Tests/Validation/Canola/Greenethorpe2013.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAD32E0-6BAB-41C8-80BF-3A83274E5090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD844B5-8002-4CBB-A03B-950EFCD174C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
+    <workbookView xWindow="-27675" yWindow="1125" windowWidth="21600" windowHeight="11280" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Canola.Stem.NConc</t>
   </si>
   <si>
-    <t>Canola.Leaf.Live.Nconc</t>
-  </si>
-  <si>
     <t>Canola.Leaf.LAI</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Clock.Today</t>
   </si>
   <si>
-    <t>treat</t>
-  </si>
-  <si>
     <t>site</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>Canola.Leaf.SpecificArea</t>
   </si>
   <si>
-    <t>Canola.Shell.Nconc</t>
-  </si>
-  <si>
     <t>Canola.DaysAfterSowing</t>
   </si>
   <si>
@@ -163,6 +154,15 @@
   </si>
   <si>
     <t>nil</t>
+  </si>
+  <si>
+    <t>Canola.Leaf.Live.NConc</t>
+  </si>
+  <si>
+    <t>Canola.Shell.NConc</t>
+  </si>
+  <si>
+    <t>Treat</t>
   </si>
 </sst>
 </file>
@@ -198,11 +198,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -261,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -367,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -509,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,7 +519,7 @@
   <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,82 +555,82 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" t="s">
         <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" t="s">
-        <v>10</v>
       </c>
       <c r="Y1" t="s">
         <v>9</v>
       </c>
       <c r="Z1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="AA1" t="s">
         <v>8</v>
@@ -660,7 +659,7 @@
       <c r="G2" s="1">
         <v>41401</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
         <f>G2-F2</f>
         <v>43</v>
       </c>
@@ -709,7 +708,7 @@
       <c r="G3" s="1">
         <v>41444</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3">
         <f t="shared" ref="H3:H29" si="1">G3-F3</f>
         <v>86</v>
       </c>
@@ -758,7 +757,7 @@
       <c r="G4" s="1">
         <v>41479</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
@@ -810,7 +809,7 @@
       <c r="G5" s="1">
         <v>41492</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
@@ -862,7 +861,7 @@
       <c r="G6" s="1">
         <v>41528</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
@@ -914,7 +913,7 @@
       <c r="G7" s="1">
         <v>41563</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>205</v>
       </c>
@@ -960,7 +959,7 @@
       <c r="G8" s="1">
         <v>41582</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
@@ -1030,7 +1029,7 @@
       <c r="G9" s="1">
         <v>41470</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
@@ -1064,7 +1063,7 @@
       <c r="G10" s="1">
         <v>41479</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -1116,7 +1115,7 @@
       <c r="G11" s="1">
         <v>41485</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
@@ -1168,7 +1167,7 @@
       <c r="G12" s="1">
         <v>41492</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
@@ -1220,7 +1219,7 @@
       <c r="G13" s="1">
         <v>41515</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1261,7 +1260,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1272,7 +1271,7 @@
       <c r="G14" s="1">
         <v>41570</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -1342,7 +1341,7 @@
       <c r="G15" s="1">
         <v>41479</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1394,7 +1393,7 @@
       <c r="G16" s="1">
         <v>41479</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1446,7 +1445,7 @@
       <c r="G17" s="1">
         <v>41479</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1498,7 +1497,7 @@
       <c r="G18" s="1">
         <v>41485</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1556,7 +1555,7 @@
       <c r="G19" s="1">
         <v>41485</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1614,7 +1613,7 @@
       <c r="G20" s="1">
         <v>41485</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -1672,7 +1671,7 @@
       <c r="G21" s="1">
         <v>41515</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1733,7 +1732,7 @@
       <c r="G22" s="1">
         <v>41515</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1783,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -1794,7 +1793,7 @@
       <c r="G23" s="1">
         <v>41515</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
@@ -1855,7 +1854,7 @@
       <c r="G24" s="1">
         <v>41543</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
@@ -1904,7 +1903,7 @@
       <c r="G25" s="1">
         <v>41543</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
@@ -1942,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
         <v>0</v>
@@ -1953,7 +1952,7 @@
       <c r="G26" s="1">
         <v>41543</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
@@ -2002,7 +2001,7 @@
       <c r="G27" s="1">
         <v>41570</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -2075,7 +2074,7 @@
       <c r="G28" s="1">
         <v>41570</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>
@@ -2148,7 +2147,7 @@
       <c r="G29" s="1">
         <v>41570</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
@@ -2200,7 +2199,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -2220,7 +2219,7 @@
       <c r="G41" s="1">
         <v>41563</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41">
         <f t="shared" ref="H41" si="2">G41-F41</f>
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
fix units of nconc obs data
</commit_message>
<xml_diff>
--- a/Tests/Validation/Canola/Greenethorpe2013.xlsx
+++ b/Tests/Validation/Canola/Greenethorpe2013.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Canola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD844B5-8002-4CBB-A03B-950EFCD174C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9FCEA7-34FA-48C6-9736-22C7B9F7CDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27675" yWindow="1125" windowWidth="21600" windowHeight="11280" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -518,42 +518,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7873D758-2B96-4EE8-A7C0-7EBF4418075C}">
   <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.59765625" customWidth="1"/>
+    <col min="11" max="11" width="23.1328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.73046875" customWidth="1"/>
+    <col min="14" max="14" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.86328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.86328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.265625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -636,7 +636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A29" si="0">B2&amp;I2&amp;C2&amp;"Cv"&amp;D2</f>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -685,7 +685,7 @@
         <v>169.28</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -734,7 +734,7 @@
         <v>207.81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -786,7 +786,7 @@
         <v>182.68</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -838,7 +838,7 @@
         <v>206.06</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -890,7 +890,7 @@
         <v>158.69</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -936,7 +936,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -1006,7 +1006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1040,7 +1040,7 @@
         <v>90.704614800000002</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1092,7 +1092,7 @@
         <v>251.83</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1144,7 +1144,7 @@
         <v>302.83999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1196,7 +1196,7 @@
         <v>286.22000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1248,7 +1248,7 @@
         <v>286.04000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola575_CL</v>
@@ -1318,7 +1318,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1370,7 +1370,7 @@
         <v>248.28</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1422,7 +1422,7 @@
         <v>227.21</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1474,7 +1474,7 @@
         <v>253.76</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1526,13 +1526,13 @@
         <v>295.52</v>
       </c>
       <c r="X18">
-        <v>6.32</v>
+        <v>6.3200000000000006E-2</v>
       </c>
       <c r="Y18">
-        <v>5.16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+        <v>5.16E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1584,13 +1584,13 @@
         <v>304.13</v>
       </c>
       <c r="X19">
-        <v>6.66</v>
+        <v>6.6600000000000006E-2</v>
       </c>
       <c r="Y19">
-        <v>5.77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+        <v>5.7699999999999994E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1642,13 +1642,13 @@
         <v>306.02999999999997</v>
       </c>
       <c r="X20">
-        <v>6.53</v>
+        <v>6.5299999999999997E-2</v>
       </c>
       <c r="Y20">
-        <v>5.43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+        <v>5.4299999999999994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1700,16 +1700,16 @@
         <v>282.43</v>
       </c>
       <c r="X21">
-        <v>5.59</v>
+        <v>5.5899999999999998E-2</v>
       </c>
       <c r="Y21">
-        <v>2.83</v>
+        <v>2.8300000000000002E-2</v>
       </c>
       <c r="AA21">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+        <v>3.2400000000000005E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1761,16 +1761,16 @@
         <v>271.61</v>
       </c>
       <c r="X22">
-        <v>6.17</v>
+        <v>6.1699999999999998E-2</v>
       </c>
       <c r="Y22">
-        <v>3.82</v>
+        <v>3.8199999999999998E-2</v>
       </c>
       <c r="AA22">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1822,16 +1822,16 @@
         <v>257.76</v>
       </c>
       <c r="X23">
-        <v>5.54</v>
+        <v>5.5399999999999998E-2</v>
       </c>
       <c r="Y23">
-        <v>2.88</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="AA23">
-        <v>3.23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+        <v>3.2300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1880,7 +1880,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1929,7 +1929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -1978,7 +1978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -2048,10 +2048,10 @@
         <v>41</v>
       </c>
       <c r="Z27">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -2121,10 +2121,10 @@
         <v>36</v>
       </c>
       <c r="Z28">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola575_CL</v>
@@ -2194,10 +2194,10 @@
         <v>41</v>
       </c>
       <c r="Z29">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -2231,7 +2231,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA29" xr:uid="{2557CFD6-CB19-4391-8652-D83569434BCC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;KFF0000 UNOFFICIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;KFF0000 UNOFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>